<commit_message>
Version 5V, Lite, and Core.
fixed spelling errors
</commit_message>
<xml_diff>
--- a/hardware/memory/Memory Map.xlsx
+++ b/hardware/memory/Memory Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jules\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EB5735-17E4-494D-9F9D-DD4F99780CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1232BC72-4A74-4B2D-881E-1494BCA41F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{373489EA-859E-4EE6-860B-453F011C26CC}"/>
   </bookViews>
@@ -3164,39 +3164,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Two switchable 4 KB </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>memory banks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, able to access 640 KB of memory, 128 KB of ROM, and 256 KB of memory mapped I/O. Offboard found/video data.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">16 x 4 KB banks of </t>
     </r>
     <r>
@@ -3279,7 +3246,51 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, able to access 64 KB of memory, 8 KB of ROM, and 8 KB of memory mapped I/O. Offboard found/video data. May be mapped to internal RAM or ROM.</t>
+      <t>, able to access 640 KB of memory, 128 KB of ROM, and 256 KB of memory mapped I/O. Offboard sound/video data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Two switchable 4 KB </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>memory banks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, able to access 64 KB of memory, 8 KB of ROM, and 8 KB of memory mapped I/O. Offboard sound/video data.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> May be mapped to internal RAM or ROM.</t>
     </r>
   </si>
 </sst>
@@ -5749,7 +5760,7 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5882,7 +5893,7 @@
       </c>
       <c r="G6" s="258"/>
       <c r="H6" s="206" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I6" s="258"/>
       <c r="J6" s="258"/>
@@ -6048,7 +6059,7 @@
       </c>
       <c r="G14" s="236"/>
       <c r="H14" s="270" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:36" s="239" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -9910,7 +9921,7 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10042,7 +10053,7 @@
         <v>384</v>
       </c>
       <c r="H6" s="102" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="77" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UPDATE: Version 5V, 5V Lite, and 5V Core.
</commit_message>
<xml_diff>
--- a/hardware/memory/Memory Map.xlsx
+++ b/hardware/memory/Memory Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jules\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1232BC72-4A74-4B2D-881E-1494BCA41F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F1BD03-7E14-4E7A-B177-DFBCA92B433A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{373489EA-859E-4EE6-860B-453F011C26CC}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="421">
   <si>
     <t>Memory Block</t>
   </si>
@@ -2878,7 +2878,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">16 x 4 KB banks of </t>
+      <t xml:space="preserve">144 x 4 KB banks of </t>
     </r>
     <r>
       <rPr>
@@ -2889,7 +2889,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>standard memory</t>
+      <t>extended memory</t>
     </r>
     <r>
       <rPr>
@@ -2903,8 +2903,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">144 x 4 KB banks of </t>
+    <t>120 KB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30 x 4 KB banks of </t>
     </r>
     <r>
       <rPr>
@@ -2915,62 +2918,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>extended memory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>120 KB</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">30 x 4 KB banks of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>extended ROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 x 4 KB banks of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>standard ROM</t>
     </r>
     <r>
       <rPr>
@@ -3291,6 +3239,84 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> May be mapped to internal RAM or ROM.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">16 x 4 KB banks of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>standard memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Pages 00 to BF map here.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 x 4 KB banks of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>standard ROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Pages E0 to FF map here.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 x 4 KB banks of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>memory mapped I/O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Pages C0 to DF map here. Device memory map partitioning determined by Southbridge.</t>
     </r>
   </si>
 </sst>
@@ -5759,8 +5785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA51CDE-CD2E-4808-9BE1-4220B016AEE8}">
   <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5893,7 +5919,7 @@
       </c>
       <c r="G6" s="258"/>
       <c r="H6" s="206" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I6" s="258"/>
       <c r="J6" s="258"/>
@@ -6059,7 +6085,7 @@
       </c>
       <c r="G14" s="236"/>
       <c r="H14" s="270" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:36" s="239" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -6075,7 +6101,7 @@
       </c>
       <c r="G15" s="236"/>
       <c r="H15" s="237" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I15" s="238"/>
       <c r="J15" s="238"/>
@@ -6116,11 +6142,11 @@
       </c>
       <c r="E16" s="272"/>
       <c r="F16" s="228" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G16" s="229"/>
       <c r="H16" s="230" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I16" s="231"/>
       <c r="J16" s="232"/>
@@ -6153,15 +6179,15 @@
       <c r="B17" s="243"/>
       <c r="C17" s="244"/>
       <c r="D17" s="227" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E17" s="272"/>
       <c r="F17" s="228" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G17" s="229"/>
       <c r="H17" s="230" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I17" s="231"/>
       <c r="J17" s="232"/>
@@ -6202,11 +6228,11 @@
       </c>
       <c r="E18" s="272"/>
       <c r="F18" s="110" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G18" s="70"/>
       <c r="H18" s="206" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="I18" s="249"/>
       <c r="J18" s="249"/>
@@ -6247,15 +6273,15 @@
       <c r="B19" s="248"/>
       <c r="C19" s="246"/>
       <c r="D19" s="252" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E19" s="273"/>
       <c r="F19" s="253" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G19" s="254"/>
       <c r="H19" s="255" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="202" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -9413,7 +9439,7 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9545,7 +9571,7 @@
         <v>384</v>
       </c>
       <c r="H6" s="102" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="77" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -9683,7 +9709,7 @@
       </c>
       <c r="G14" s="109"/>
       <c r="H14" s="200" t="s">
-        <v>400</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="239" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -9699,7 +9725,7 @@
       </c>
       <c r="G15" s="236"/>
       <c r="H15" s="237" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I15" s="238"/>
       <c r="J15" s="238"/>
@@ -9740,11 +9766,11 @@
       </c>
       <c r="E16" s="195"/>
       <c r="F16" s="77" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G16" s="197"/>
       <c r="H16" s="78" t="s">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="I16" s="215"/>
       <c r="J16" s="216"/>
@@ -9777,15 +9803,15 @@
       <c r="B17" s="224"/>
       <c r="C17" s="226"/>
       <c r="D17" s="227" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E17" s="195"/>
       <c r="F17" s="228" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G17" s="229"/>
       <c r="H17" s="230" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I17" s="231"/>
       <c r="J17" s="232"/>
@@ -9826,11 +9852,11 @@
       </c>
       <c r="E18" s="195"/>
       <c r="F18" s="110" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G18" s="70"/>
       <c r="H18" s="206" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I18" s="249"/>
       <c r="J18" s="249"/>
@@ -9871,15 +9897,15 @@
       <c r="B19" s="248"/>
       <c r="C19" s="246"/>
       <c r="D19" s="252" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E19" s="196"/>
       <c r="F19" s="253" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G19" s="254"/>
       <c r="H19" s="255" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="202" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -9921,7 +9947,7 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10053,7 +10079,7 @@
         <v>384</v>
       </c>
       <c r="H6" s="102" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="77" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -10191,7 +10217,7 @@
       </c>
       <c r="G14" s="109"/>
       <c r="H14" s="200" t="s">
-        <v>400</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="201" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10207,7 +10233,7 @@
       </c>
       <c r="G15" s="109"/>
       <c r="H15" s="217" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I15" s="218"/>
       <c r="J15" s="218"/>
@@ -10248,11 +10274,11 @@
       </c>
       <c r="E16" s="195"/>
       <c r="F16" s="77" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G16" s="197"/>
       <c r="H16" s="78" t="s">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="I16" s="215"/>
       <c r="J16" s="216"/>
@@ -10285,15 +10311,15 @@
       <c r="B17" s="224"/>
       <c r="C17" s="226"/>
       <c r="D17" s="210" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E17" s="195"/>
       <c r="F17" s="77" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G17" s="197"/>
       <c r="H17" s="78" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I17" s="215"/>
       <c r="J17" s="216"/>
@@ -10334,11 +10360,11 @@
       </c>
       <c r="E18" s="195"/>
       <c r="F18" s="110" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G18" s="70"/>
       <c r="H18" s="206" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I18" s="249"/>
       <c r="J18" s="249"/>
@@ -10379,15 +10405,15 @@
       <c r="B19" s="248"/>
       <c r="C19" s="246"/>
       <c r="D19" s="251" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E19" s="196"/>
       <c r="F19" s="103" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G19" s="67"/>
       <c r="H19" s="104" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="202" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>